<commit_message>
starting to finding more primary keys for the proponentes
</commit_message>
<xml_diff>
--- a/PowerBI_Dataset/xlsx/df_ic.xlsx
+++ b/PowerBI_Dataset/xlsx/df_ic.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>mes</t>
   </si>
@@ -27,47 +27,14 @@
   <si>
     <t>observacao</t>
   </si>
-  <si>
-    <t>Janeiro</t>
-  </si>
-  <si>
-    <t>Fevereiro</t>
-  </si>
-  <si>
-    <t>Março</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Maio</t>
-  </si>
-  <si>
-    <t>Junho</t>
-  </si>
-  <si>
-    <t>Julho</t>
-  </si>
-  <si>
-    <t>Agosto</t>
-  </si>
-  <si>
-    <t>Setembro</t>
-  </si>
-  <si>
-    <t>Outubro</t>
-  </si>
-  <si>
-    <t>Novembro</t>
-  </si>
-  <si>
-    <t>Dezembro</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -120,11 +87,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,8 +411,8 @@
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2" s="2">
+        <v>44197</v>
       </c>
       <c r="C2">
         <v>0.010077366936968</v>
@@ -457,8 +425,8 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
+      <c r="B3" s="2">
+        <v>44228</v>
       </c>
       <c r="C3">
         <v>0.010036826026</v>
@@ -471,8 +439,8 @@
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="B4" s="2">
+        <v>44256</v>
       </c>
       <c r="C4">
         <v>0.0100810659704667</v>
@@ -485,8 +453,8 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="B5" s="2">
+        <v>44287</v>
       </c>
       <c r="C5">
         <v>0.0100699729413185</v>
@@ -499,8 +467,8 @@
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
+      <c r="B6" s="2">
+        <v>44317</v>
       </c>
       <c r="C6">
         <v>0.0100810659704667</v>
@@ -513,8 +481,8 @@
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
+      <c r="B7" s="2">
+        <v>44348</v>
       </c>
       <c r="C7">
         <v>0.0100810659704667</v>
@@ -527,8 +495,8 @@
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>10</v>
+      <c r="B8" s="2">
+        <v>44378</v>
       </c>
       <c r="C8">
         <v>0.010077366936968</v>
@@ -541,8 +509,8 @@
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
+      <c r="B9" s="2">
+        <v>44409</v>
       </c>
       <c r="C9">
         <v>0.0100847663617456</v>
@@ -555,8 +523,8 @@
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>12</v>
+      <c r="B10" s="2">
+        <v>44440</v>
       </c>
       <c r="C10">
         <v>0.010077366936968</v>
@@ -569,8 +537,8 @@
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>13</v>
+      <c r="B11" s="2">
+        <v>44470</v>
       </c>
       <c r="C11">
         <v>0.0100736692607513</v>
@@ -583,16 +551,16 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="B12" s="2">
+        <v>44501</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>15</v>
+      <c r="B13" s="2">
+        <v>44531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>